<commit_message>
Updated README with report link
</commit_message>
<xml_diff>
--- a/Simulation Values.xlsx
+++ b/Simulation Values.xlsx
@@ -445,7 +445,7 @@
   <dimension ref="A1:M118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+      <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1581,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1">
+        <f>0.0248*60</f>
+        <v>1.488</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -4097,6 +4100,10 @@
         <f>AVERAGE(D109:D111)</f>
         <v>0.43039105745241235</v>
       </c>
+      <c r="F112">
+        <f>60* 0.0116</f>
+        <v>0.69599999999999995</v>
+      </c>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>

</xml_diff>